<commit_message>
Mise En Commun Joshua
</commit_message>
<xml_diff>
--- a/Journée d'activité/Constantin.xlsx
+++ b/Journée d'activité/Constantin.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3F0C74-78C5-460A-87DE-58022A916860}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E728CC80-B1B3-4C70-A10A-1E73758104F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="165" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DATE</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Choix du templates / Compréhension du templates / Reflexion sur le templates</t>
+  </si>
+  <si>
+    <t>Etude de la page Game.html / architecture détaillé du programme</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
   <dimension ref="B1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C7" sqref="C7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,8 +592,12 @@
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="13">
+        <v>43784</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -824,6 +831,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:H28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:H30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:H32"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:H22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:H24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:H26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:H16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:H18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:H20"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:H10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:H12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:H14"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:H8"/>
     <mergeCell ref="C2:H2"/>
@@ -831,30 +862,6 @@
     <mergeCell ref="C3:H4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:H6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:H10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:H14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:H16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:H18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:H20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:H22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:H24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:H26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:H28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:H30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>